<commit_message>
feat：update change animal guid
</commit_message>
<xml_diff>
--- a/dragon-verse/Excels/AnimalEcology_动物生态表.xlsx
+++ b/dragon-verse/Excels/AnimalEcology_动物生态表.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="51">
   <si>
     <t>int</t>
   </si>
@@ -135,9 +135,6 @@
     <t>3|2|5</t>
   </si>
   <si>
-    <t>4F89DF024353D4AAA93987A8FF8B9FBD</t>
-  </si>
-  <si>
     <t>TestAnimalName0002</t>
   </si>
   <si>
@@ -150,9 +147,6 @@
     <t>2|3|1</t>
   </si>
   <si>
-    <t>FAE2BD3F428A66CF8E0A88802492AD8A</t>
-  </si>
-  <si>
     <t>TestAnimalName0003</t>
   </si>
   <si>
@@ -162,9 +156,6 @@
     <t>1|2|3</t>
   </si>
   <si>
-    <t>B434BF4A4218D8FE2B4536BEFA893AA9</t>
-  </si>
-  <si>
     <t>TestAnimalName0004</t>
   </si>
   <si>
@@ -172,9 +163,6 @@
   </si>
   <si>
     <t>3|21</t>
-  </si>
-  <si>
-    <t>4C46C84046B0E75EF1A2CC91B0298D40</t>
   </si>
   <si>
     <t>-3090|-6200|990||-3533|-5161|1131||-4460|-3301|1337||-4038|-5173|1202</t>
@@ -1127,7 +1115,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="TableStylePreset3_Accent1 1" pivot="0" count="7" xr9:uid="{E592AEDA-A341-4765-8277-CC8DB018BBD4}">
+    <tableStyle name="TableStylePreset3_Accent1 1" pivot="0" count="7" xr9:uid="{F133A59C-9EC5-4852-8DFC-6C60BF004223}">
       <tableStyleElement type="wholeTable" dxfId="6"/>
       <tableStyleElement type="headerRow" dxfId="5"/>
       <tableStyleElement type="totalRow" dxfId="4"/>
@@ -1136,7 +1124,7 @@
       <tableStyleElement type="firstRowStripe" dxfId="1"/>
       <tableStyleElement type="firstColumnStripe" dxfId="0"/>
     </tableStyle>
-    <tableStyle name="PivotStylePreset2_Accent1 1" table="0" count="10" xr9:uid="{D411F081-E5C7-464D-A04D-36BAD90D6E57}">
+    <tableStyle name="PivotStylePreset2_Accent1 1" table="0" count="10" xr9:uid="{704AE7F2-5DB9-4ED7-BB11-0A9FF04E69F2}">
       <tableStyleElement type="headerRow" dxfId="16"/>
       <tableStyleElement type="totalRow" dxfId="15"/>
       <tableStyleElement type="firstRowStripe" dxfId="14"/>
@@ -1393,8 +1381,8 @@
   <sheetPr/>
   <dimension ref="A1:M301"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="16.5"/>
@@ -1578,8 +1566,8 @@
       <c r="L5" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="M5" s="3" t="s">
-        <v>33</v>
+      <c r="M5" s="3">
+        <v>159590</v>
       </c>
     </row>
     <row r="6" s="3" customFormat="1" spans="1:13">
@@ -1587,14 +1575,14 @@
         <v>2</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" s="8" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B6,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D6" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E6" s="2">
         <v>0</v>
@@ -1615,13 +1603,13 @@
         <v>1</v>
       </c>
       <c r="K6" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="L6" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>38</v>
+      <c r="M6" s="3">
+        <v>159750</v>
       </c>
     </row>
     <row r="7" s="3" customFormat="1" spans="1:13">
@@ -1629,14 +1617,14 @@
         <v>3</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C7" s="8" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B7,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D7" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E7" s="2">
         <v>0</v>
@@ -1657,13 +1645,13 @@
         <v>1</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
+      </c>
+      <c r="M7" s="3">
+        <v>159842</v>
       </c>
     </row>
     <row r="8" s="3" customFormat="1" spans="1:13">
@@ -1671,14 +1659,14 @@
         <v>4</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C8" s="8" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B8,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D8" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E8" s="2">
         <v>0</v>
@@ -1699,13 +1687,13 @@
         <v>1</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>46</v>
+        <v>39</v>
+      </c>
+      <c r="M8" s="3">
+        <v>160045</v>
       </c>
     </row>
     <row r="9" s="3" customFormat="1" spans="1:13">
@@ -1720,7 +1708,7 @@
         <v/>
       </c>
       <c r="D9" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E9" s="2">
         <v>60000</v>
@@ -1746,8 +1734,8 @@
       <c r="L9" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="M9" s="3" t="s">
-        <v>33</v>
+      <c r="M9" s="3">
+        <v>159590</v>
       </c>
     </row>
     <row r="10" s="3" customFormat="1" spans="1:13">
@@ -1755,14 +1743,14 @@
         <v>6</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="8" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B10,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D10" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E10" s="2">
         <v>60000</v>
@@ -1783,13 +1771,13 @@
         <v>1</v>
       </c>
       <c r="K10" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="L10" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="L10" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>38</v>
+      <c r="M10" s="3">
+        <v>159750</v>
       </c>
     </row>
     <row r="11" s="3" customFormat="1" spans="1:13">
@@ -1797,14 +1785,14 @@
         <v>7</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C11" s="8" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B11,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D11" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E11" s="2">
         <v>60000</v>
@@ -1825,13 +1813,13 @@
         <v>1</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L11" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
+      </c>
+      <c r="M11" s="3">
+        <v>159842</v>
       </c>
     </row>
     <row r="12" s="3" customFormat="1" spans="1:13">
@@ -1839,14 +1827,14 @@
         <v>8</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C12" s="8" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B12,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D12" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E12" s="2">
         <v>60000</v>
@@ -1867,13 +1855,13 @@
         <v>1</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="L12" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>46</v>
+        <v>39</v>
+      </c>
+      <c r="M12" s="3">
+        <v>160045</v>
       </c>
     </row>
     <row r="13" s="3" customFormat="1" spans="1:13">
@@ -1888,7 +1876,7 @@
         <v/>
       </c>
       <c r="D13" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E13" s="2">
         <v>120000</v>
@@ -1914,8 +1902,8 @@
       <c r="L13" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="M13" s="3" t="s">
-        <v>33</v>
+      <c r="M13" s="3">
+        <v>159590</v>
       </c>
     </row>
     <row r="14" s="3" customFormat="1" spans="1:13">
@@ -1923,14 +1911,14 @@
         <v>10</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" s="8" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B14,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D14" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E14" s="2">
         <v>120000</v>
@@ -1951,13 +1939,13 @@
         <v>1</v>
       </c>
       <c r="K14" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="L14" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="L14" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="M14" s="3" t="s">
-        <v>38</v>
+      <c r="M14" s="3">
+        <v>159750</v>
       </c>
     </row>
     <row r="15" s="3" customFormat="1" spans="1:13">
@@ -1965,14 +1953,14 @@
         <v>11</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C15" s="8" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B15,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D15" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E15" s="2">
         <v>120000</v>
@@ -1993,13 +1981,13 @@
         <v>1</v>
       </c>
       <c r="K15" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L15" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
+      </c>
+      <c r="M15" s="3">
+        <v>159842</v>
       </c>
     </row>
     <row r="16" s="3" customFormat="1" spans="2:7">
@@ -3847,7 +3835,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1">
         <v>1000</v>

</xml_diff>

<commit_message>
feat：update animEcology and level change
</commit_message>
<xml_diff>
--- a/dragon-verse/Excels/AnimalEcology_动物生态表.xlsx
+++ b/dragon-verse/Excels/AnimalEcology_动物生态表.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
   <si>
     <t>int</t>
   </si>
@@ -132,10 +132,10 @@
     <t>TestAnimalName0001</t>
   </si>
   <si>
-    <t>29|33</t>
-  </si>
-  <si>
-    <t>3|2|5</t>
+    <t>29|33|39</t>
+  </si>
+  <si>
+    <t>5|3|6</t>
   </si>
   <si>
     <t>150833|150830|150834</t>
@@ -144,13 +144,13 @@
     <t>TestAnimalName0002</t>
   </si>
   <si>
-    <t>30|34</t>
-  </si>
-  <si>
-    <t>2|1|3</t>
-  </si>
-  <si>
-    <t>2|3|1</t>
+    <t>30|34|40</t>
+  </si>
+  <si>
+    <t>100|300|500</t>
+  </si>
+  <si>
+    <t>3|4|5</t>
   </si>
   <si>
     <t>181301|181390|235648</t>
@@ -159,10 +159,10 @@
     <t>TestAnimalName0003</t>
   </si>
   <si>
-    <t>31|35</t>
-  </si>
-  <si>
-    <t>1|2|3</t>
+    <t>31|35|41</t>
+  </si>
+  <si>
+    <t>3|2|4</t>
   </si>
   <si>
     <t>TestAnimalName0004</t>
@@ -171,16 +171,7 @@
     <t>32|38</t>
   </si>
   <si>
-    <t>3|21</t>
-  </si>
-  <si>
-    <t>1731|7838|1564||-66|7976|1553||6303|3548|1691</t>
-  </si>
-  <si>
-    <t>-11272|6585|3358||-9615|9185|3873||5035|5120|1652</t>
-  </si>
-  <si>
-    <t>-10249|441|2078||-8841|-1131|1679||-11098|1544|2448</t>
+    <t>2|3|4</t>
   </si>
   <si>
     <t>MaxLanItemCount</t>
@@ -1102,7 +1093,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="TableStylePreset3_Accent1 1" pivot="0" count="7" xr9:uid="{FC8FE73F-2AD6-4A42-9FB7-C3913E977C61}">
+    <tableStyle name="TableStylePreset3_Accent1 1" pivot="0" count="7" xr9:uid="{972126A5-96AD-4B8C-A428-6E94522F919A}">
       <tableStyleElement type="wholeTable" dxfId="6"/>
       <tableStyleElement type="headerRow" dxfId="5"/>
       <tableStyleElement type="totalRow" dxfId="4"/>
@@ -1111,7 +1102,7 @@
       <tableStyleElement type="firstRowStripe" dxfId="1"/>
       <tableStyleElement type="firstColumnStripe" dxfId="0"/>
     </tableStyle>
-    <tableStyle name="PivotStylePreset2_Accent1 1" table="0" count="10" xr9:uid="{A8CE8836-D93D-4677-A432-BD6980C157C5}">
+    <tableStyle name="PivotStylePreset2_Accent1 1" table="0" count="10" xr9:uid="{DB1E98DD-09C4-430F-80C3-6A4334D0CBDE}">
       <tableStyleElement type="headerRow" dxfId="16"/>
       <tableStyleElement type="totalRow" dxfId="15"/>
       <tableStyleElement type="firstRowStripe" dxfId="14"/>
@@ -1355,10 +1346,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M301"/>
+  <dimension ref="A1:M294"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="16.5"/>
@@ -1522,19 +1513,19 @@
         <v>0</v>
       </c>
       <c r="F5" s="2">
-        <v>60000</v>
+        <v>300000</v>
       </c>
       <c r="G5" s="2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H5" s="2">
-        <v>60000</v>
+        <v>300000</v>
       </c>
       <c r="I5" s="2">
-        <v>500</v>
+        <v>5000</v>
       </c>
       <c r="J5" s="2">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>33</v>
@@ -1564,16 +1555,16 @@
         <v>0</v>
       </c>
       <c r="F6" s="2">
-        <v>60000</v>
+        <v>300000</v>
       </c>
       <c r="G6" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H6" s="2">
-        <v>60000</v>
+        <v>300000</v>
       </c>
       <c r="I6" s="2">
-        <v>500</v>
+        <v>5000</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>37</v>
@@ -1606,19 +1597,19 @@
         <v>0</v>
       </c>
       <c r="F7" s="2">
-        <v>60000</v>
+        <v>300000</v>
       </c>
       <c r="G7" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H7" s="2">
-        <v>60000</v>
+        <v>300000</v>
       </c>
       <c r="I7" s="2">
-        <v>500</v>
+        <v>5000</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>42</v>
@@ -1645,315 +1636,124 @@
         <v>0</v>
       </c>
       <c r="F8" s="2">
-        <v>60000</v>
+        <v>300000</v>
       </c>
       <c r="G8" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H8" s="2">
-        <v>60000</v>
+        <v>300000</v>
       </c>
       <c r="I8" s="2">
-        <v>500</v>
+        <v>5000</v>
       </c>
       <c r="J8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K8" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="L8" s="3">
         <v>160045</v>
       </c>
     </row>
-    <row r="9" s="3" customFormat="1" spans="1:12">
-      <c r="A9" s="3">
-        <v>5</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>31</v>
-      </c>
+    <row r="9" s="3" customFormat="1" spans="2:7">
+      <c r="B9" s="8"/>
       <c r="C9" s="8" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B9,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D9" s="4"/>
-      <c r="E9" s="2">
-        <v>60000</v>
-      </c>
-      <c r="F9" s="2">
-        <v>60000</v>
-      </c>
-      <c r="G9" s="2">
-        <v>1</v>
-      </c>
-      <c r="H9" s="2">
-        <v>60000</v>
-      </c>
-      <c r="I9" s="2">
-        <v>500</v>
-      </c>
-      <c r="J9" s="2">
-        <v>1</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="L9" s="3">
-        <v>159590</v>
-      </c>
-    </row>
-    <row r="10" s="3" customFormat="1" spans="1:12">
-      <c r="A10" s="3">
-        <v>6</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>35</v>
-      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" s="3" customFormat="1" spans="2:7">
+      <c r="B10" s="8"/>
       <c r="C10" s="8" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B10,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D10" s="4"/>
-      <c r="E10" s="2">
-        <v>60000</v>
-      </c>
-      <c r="F10" s="2">
-        <v>60000</v>
-      </c>
-      <c r="G10" s="2">
-        <v>2</v>
-      </c>
-      <c r="H10" s="2">
-        <v>60000</v>
-      </c>
-      <c r="I10" s="2">
-        <v>500</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L10" s="3">
-        <v>159750</v>
-      </c>
-    </row>
-    <row r="11" s="3" customFormat="1" spans="1:12">
-      <c r="A11" s="3">
-        <v>7</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>40</v>
-      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" s="3" customFormat="1" spans="1:7">
+      <c r="A11" s="10"/>
+      <c r="B11" s="8"/>
       <c r="C11" s="8" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B11,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D11" s="4"/>
-      <c r="E11" s="2">
-        <v>60000</v>
-      </c>
-      <c r="F11" s="2">
-        <v>60000</v>
-      </c>
-      <c r="G11" s="2">
-        <v>2</v>
-      </c>
-      <c r="H11" s="2">
-        <v>60000</v>
-      </c>
-      <c r="I11" s="2">
-        <v>500</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L11" s="3">
-        <v>159842</v>
-      </c>
-    </row>
-    <row r="12" s="3" customFormat="1" spans="1:12">
-      <c r="A12" s="3">
-        <v>8</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>43</v>
-      </c>
+      <c r="E11" s="9"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" s="3" customFormat="1" spans="1:7">
+      <c r="A12" s="10"/>
+      <c r="B12" s="8"/>
       <c r="C12" s="8" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B12,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D12" s="4"/>
-      <c r="E12" s="2">
-        <v>60000</v>
-      </c>
-      <c r="F12" s="2">
-        <v>60000</v>
-      </c>
-      <c r="G12" s="2">
-        <v>1</v>
-      </c>
-      <c r="H12" s="2">
-        <v>60000</v>
-      </c>
-      <c r="I12" s="2">
-        <v>500</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L12" s="3">
-        <v>160045</v>
-      </c>
-    </row>
-    <row r="13" s="3" customFormat="1" spans="1:12">
-      <c r="A13" s="3">
-        <v>9</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>31</v>
-      </c>
+      <c r="E12" s="9"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" s="3" customFormat="1" spans="1:5">
+      <c r="A13" s="10"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="8" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B13,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="2">
-        <v>120000</v>
-      </c>
-      <c r="F13" s="2">
-        <v>60000</v>
-      </c>
-      <c r="G13" s="2">
-        <v>2</v>
-      </c>
-      <c r="H13" s="2">
-        <v>60000</v>
-      </c>
-      <c r="I13" s="2">
-        <v>500</v>
-      </c>
-      <c r="J13" s="2">
-        <v>1</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="L13" s="3">
-        <v>159590</v>
-      </c>
-    </row>
-    <row r="14" s="3" customFormat="1" spans="1:12">
-      <c r="A14" s="3">
-        <v>10</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>35</v>
-      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" s="3" customFormat="1" spans="1:5">
+      <c r="A14" s="10"/>
+      <c r="B14" s="8"/>
       <c r="C14" s="8" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B14,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="2">
-        <v>120000</v>
-      </c>
-      <c r="F14" s="2">
-        <v>60000</v>
-      </c>
-      <c r="G14" s="2">
-        <v>2</v>
-      </c>
-      <c r="H14" s="2">
-        <v>60000</v>
-      </c>
-      <c r="I14" s="2">
-        <v>500</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L14" s="3">
-        <v>159750</v>
-      </c>
-    </row>
-    <row r="15" s="3" customFormat="1" spans="1:12">
-      <c r="A15" s="3">
-        <v>11</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>40</v>
-      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" s="3" customFormat="1" spans="1:5">
+      <c r="A15" s="10"/>
+      <c r="B15" s="8"/>
       <c r="C15" s="8" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B15,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" s="2">
-        <v>120000</v>
-      </c>
-      <c r="F15" s="2">
-        <v>60000</v>
-      </c>
-      <c r="G15" s="9">
-        <v>2</v>
-      </c>
-      <c r="H15" s="2">
-        <v>60000</v>
-      </c>
-      <c r="I15" s="2">
-        <v>500</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L15" s="3">
-        <v>159842</v>
-      </c>
-    </row>
-    <row r="16" s="3" customFormat="1" spans="2:7">
+      <c r="D15" s="4"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" s="3" customFormat="1" spans="1:5">
+      <c r="A16" s="10"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B16,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D16" s="4"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-    </row>
-    <row r="17" s="3" customFormat="1" spans="2:7">
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" s="3" customFormat="1" spans="1:5">
+      <c r="A17" s="10"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B17,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
       <c r="D17" s="4"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-    </row>
-    <row r="18" s="3" customFormat="1" spans="1:7">
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" s="3" customFormat="1" spans="1:5">
       <c r="A18" s="10"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8" t="str">
@@ -1961,11 +1761,9 @@
         <v/>
       </c>
       <c r="D18" s="4"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-    </row>
-    <row r="19" s="3" customFormat="1" spans="1:7">
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" s="3" customFormat="1" spans="1:5">
       <c r="A19" s="10"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8" t="str">
@@ -1973,13 +1771,10 @@
         <v/>
       </c>
       <c r="D19" s="4"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
+      <c r="E19" s="2"/>
     </row>
     <row r="20" s="3" customFormat="1" spans="1:5">
       <c r="A20" s="10"/>
-      <c r="B20" s="8"/>
       <c r="C20" s="8" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B20,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
@@ -1989,7 +1784,6 @@
     </row>
     <row r="21" s="3" customFormat="1" spans="1:5">
       <c r="A21" s="10"/>
-      <c r="B21" s="8"/>
       <c r="C21" s="8" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B21,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
@@ -1999,7 +1793,6 @@
     </row>
     <row r="22" s="3" customFormat="1" spans="1:5">
       <c r="A22" s="10"/>
-      <c r="B22" s="8"/>
       <c r="C22" s="8" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B22,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
@@ -2009,7 +1802,6 @@
     </row>
     <row r="23" s="3" customFormat="1" spans="1:5">
       <c r="A23" s="10"/>
-      <c r="B23" s="8"/>
       <c r="C23" s="8" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B23,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
@@ -2019,7 +1811,6 @@
     </row>
     <row r="24" s="3" customFormat="1" spans="1:5">
       <c r="A24" s="10"/>
-      <c r="B24" s="8"/>
       <c r="C24" s="8" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B24,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
@@ -2029,7 +1820,6 @@
     </row>
     <row r="25" s="3" customFormat="1" spans="1:5">
       <c r="A25" s="10"/>
-      <c r="B25" s="8"/>
       <c r="C25" s="8" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B25,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
@@ -2039,7 +1829,6 @@
     </row>
     <row r="26" s="3" customFormat="1" spans="1:5">
       <c r="A26" s="10"/>
-      <c r="B26" s="8"/>
       <c r="C26" s="8" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B26,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
@@ -2137,8 +1926,7 @@
       <c r="D36" s="4"/>
       <c r="E36" s="2"/>
     </row>
-    <row r="37" s="3" customFormat="1" spans="1:5">
-      <c r="A37" s="10"/>
+    <row r="37" s="3" customFormat="1" spans="3:5">
       <c r="C37" s="8" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B37,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
@@ -2146,82 +1934,62 @@
       <c r="D37" s="4"/>
       <c r="E37" s="2"/>
     </row>
-    <row r="38" s="3" customFormat="1" spans="1:5">
-      <c r="A38" s="10"/>
+    <row r="38" spans="3:3">
       <c r="C38" s="8" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B38,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D38" s="4"/>
-      <c r="E38" s="2"/>
-    </row>
-    <row r="39" s="3" customFormat="1" spans="1:5">
-      <c r="A39" s="10"/>
+    </row>
+    <row r="39" spans="3:3">
       <c r="C39" s="8" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B39,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D39" s="4"/>
-      <c r="E39" s="2"/>
-    </row>
-    <row r="40" s="3" customFormat="1" spans="1:5">
-      <c r="A40" s="10"/>
+    </row>
+    <row r="40" spans="3:3">
       <c r="C40" s="8" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B40,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D40" s="4"/>
-      <c r="E40" s="2"/>
-    </row>
-    <row r="41" s="3" customFormat="1" spans="1:5">
-      <c r="A41" s="10"/>
-      <c r="C41" s="8" t="str">
+    </row>
+    <row r="41" spans="3:3">
+      <c r="C41" s="3" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B41,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D41" s="4"/>
-      <c r="E41" s="2"/>
-    </row>
-    <row r="42" s="3" customFormat="1" spans="1:5">
-      <c r="A42" s="10"/>
-      <c r="C42" s="8" t="str">
+    </row>
+    <row r="42" spans="3:3">
+      <c r="C42" s="3" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B42,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D42" s="4"/>
-      <c r="E42" s="2"/>
-    </row>
-    <row r="43" s="3" customFormat="1" spans="1:5">
-      <c r="A43" s="10"/>
-      <c r="C43" s="8" t="str">
+    </row>
+    <row r="43" spans="3:3">
+      <c r="C43" s="3" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B43,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D43" s="4"/>
-      <c r="E43" s="2"/>
-    </row>
-    <row r="44" s="3" customFormat="1" spans="3:5">
-      <c r="C44" s="8" t="str">
+    </row>
+    <row r="44" spans="3:3">
+      <c r="C44" s="3" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B44,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D44" s="4"/>
-      <c r="E44" s="2"/>
     </row>
     <row r="45" spans="3:3">
-      <c r="C45" s="8" t="str">
+      <c r="C45" s="3" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B45,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="46" spans="3:3">
-      <c r="C46" s="8" t="str">
+      <c r="C46" s="3" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B46,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
     <row r="47" spans="3:3">
-      <c r="C47" s="8" t="str">
+      <c r="C47" s="3" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B47,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
@@ -3705,48 +3473,6 @@
     <row r="294" spans="3:3">
       <c r="C294" s="3" t="str">
         <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B294,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="295" spans="3:3">
-      <c r="C295" s="3" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B295,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="296" spans="3:3">
-      <c r="C296" s="3" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B296,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="297" spans="3:3">
-      <c r="C297" s="3" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B297,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="298" spans="3:3">
-      <c r="C298" s="3" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B298,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="299" spans="3:3">
-      <c r="C299" s="3" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B299,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="300" spans="3:3">
-      <c r="C300" s="3" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B300,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="301" spans="3:3">
-      <c r="C301" s="3" t="str">
-        <f ca="1">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B301,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
     </row>
@@ -3776,7 +3502,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B1" s="1">
         <v>1000</v>

</xml_diff>